<commit_message>
Switched to 2025 Feb
</commit_message>
<xml_diff>
--- a/data/stata-licenses-by-country.xlsx
+++ b/data/stata-licenses-by-country.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Stata" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">Country</t>
   </si>
@@ -31,25 +31,50 @@
     <t xml:space="preserve">Stata license</t>
   </si>
   <si>
-    <t xml:space="preserve">Percent</t>
+    <t xml:space="preserve">Laptop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Currency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exchange rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laptop USD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent license</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent laptop</t>
   </si>
   <si>
     <t xml:space="preserve">USA</t>
   </si>
   <si>
+    <t xml:space="preserve">USD</t>
+  </si>
+  <si>
     <t xml:space="preserve">Greece</t>
   </si>
   <si>
+    <t xml:space="preserve">EUR</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vietnam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0%"/>
+    <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="0%"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -115,16 +140,28 @@
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -317,71 +354,141 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2:D4"/>
+      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.60546875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.83"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="0" t="n">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="n">
         <v>6704</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>690</v>
       </c>
       <c r="D2" s="1" t="n">
+        <v>849</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <f aca="false">D2</f>
+        <v>849</v>
+      </c>
+      <c r="H2" s="3" t="n">
         <f aca="false">C2/B2*100</f>
         <v>10.2923627684964</v>
       </c>
+      <c r="I2" s="4" t="n">
+        <f aca="false">G2/B2*100</f>
+        <v>12.6640811455847</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="0" t="n">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="n">
         <v>1883</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>690</v>
       </c>
       <c r="D3" s="1" t="n">
+        <v>799</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <f aca="false">D3*F3</f>
+        <v>934.83</v>
+      </c>
+      <c r="H3" s="3" t="n">
         <f aca="false">C3/B3*100</f>
         <v>36.6436537440255</v>
       </c>
+      <c r="I3" s="4" t="n">
+        <f aca="false">G3/B3*100</f>
+        <v>49.6457780138078</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="0" t="n">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="n">
         <v>343</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>220</v>
       </c>
       <c r="D4" s="1" t="n">
+        <v>18440000</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>38.32</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <f aca="false">D4/1000000*F4</f>
+        <v>706.6208</v>
+      </c>
+      <c r="H4" s="3" t="n">
         <f aca="false">C4/B4*100</f>
         <v>64.1399416909621</v>
+      </c>
+      <c r="I4" s="4" t="n">
+        <f aca="false">G4/B4*100</f>
+        <v>206.011895043732</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjusting table with laptop prices
</commit_message>
<xml_diff>
--- a/data/stata-licenses-by-country.xlsx
+++ b/data/stata-licenses-by-country.xlsx
@@ -73,7 +73,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="[$$-409]#,##0;[RED]\-[$$-409]#,##0"/>
     <numFmt numFmtId="166" formatCode="0%"/>
   </numFmts>
   <fonts count="4">
@@ -144,24 +144,28 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -357,136 +361,136 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.60546875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="3" t="n">
         <v>6704</v>
       </c>
-      <c r="C2" s="1" t="n">
+      <c r="C2" s="3" t="n">
         <v>690</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" s="2" t="n">
         <v>849</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="1" t="n">
+      <c r="F2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="G2" s="4" t="n">
         <f aca="false">D2</f>
         <v>849</v>
       </c>
-      <c r="H2" s="3" t="n">
+      <c r="H2" s="5" t="n">
         <f aca="false">C2/B2*100</f>
         <v>10.2923627684964</v>
       </c>
-      <c r="I2" s="4" t="n">
+      <c r="I2" s="1" t="n">
         <f aca="false">G2/B2*100</f>
         <v>12.6640811455847</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B3" s="3" t="n">
         <v>1883</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="C3" s="3" t="n">
         <v>690</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="D3" s="2" t="n">
         <v>799</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="1" t="n">
+      <c r="F3" s="2" t="n">
         <v>1.17</v>
       </c>
-      <c r="G3" s="2" t="n">
+      <c r="G3" s="4" t="n">
         <f aca="false">D3*F3</f>
         <v>934.83</v>
       </c>
-      <c r="H3" s="3" t="n">
+      <c r="H3" s="5" t="n">
         <f aca="false">C3/B3*100</f>
         <v>36.6436537440255</v>
       </c>
-      <c r="I3" s="4" t="n">
+      <c r="I3" s="1" t="n">
         <f aca="false">G3/B3*100</f>
         <v>49.6457780138078</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B4" s="3" t="n">
         <v>343</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="C4" s="3" t="n">
         <v>220</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="D4" s="2" t="n">
         <v>18440000</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="1" t="n">
+      <c r="F4" s="2" t="n">
         <v>38.32</v>
       </c>
-      <c r="G4" s="2" t="n">
+      <c r="G4" s="4" t="n">
         <f aca="false">D4/1000000*F4</f>
         <v>706.6208</v>
       </c>
-      <c r="H4" s="3" t="n">
+      <c r="H4" s="5" t="n">
         <f aca="false">C4/B4*100</f>
         <v>64.1399416909621</v>
       </c>
-      <c r="I4" s="4" t="n">
+      <c r="I4" s="1" t="n">
         <f aca="false">G4/B4*100</f>
         <v>206.011895043732</v>
       </c>

</xml_diff>